<commit_message>
Pruebas 001 añadidas - NBQ_050100
</commit_message>
<xml_diff>
--- a/ControlCambios/07_Pruebas/Pruebas_001.xlsx
+++ b/ControlCambios/07_Pruebas/Pruebas_001.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nubeusc-my.sharepoint.com/personal/roi_martinez_enriquez_rai_usc_es/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niko\Documents\Uni\EnSo\EnSo_ControlCambios_gr1.2\ControlCambios\07_Pruebas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C7CDA229-CBF5-4818-9FB4-F78E3B9AAD6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17675671-0B41-4A8A-B8BD-DD8B8FE7DDA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{76D02679-E598-4CD7-BD3A-2F54FDE5D7B6}"/>
+    <workbookView xWindow="9336" yWindow="0" windowWidth="13800" windowHeight="12336" xr2:uid="{76D02679-E598-4CD7-BD3A-2F54FDE5D7B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Pruebas" sheetId="1" r:id="rId1"/>
@@ -59,21 +59,12 @@
     <t>Nombre</t>
   </si>
   <si>
-    <t>[Nombre completo del responsable de las pruebas]</t>
-  </si>
-  <si>
     <t>Correo</t>
   </si>
   <si>
-    <t xml:space="preserve"> [Correo electrónico del responsable]</t>
-  </si>
-  <si>
     <t>ID del empleado</t>
   </si>
   <si>
-    <t xml:space="preserve">[ID del empleado] </t>
-  </si>
-  <si>
     <t>Resultados de Pruebas</t>
   </si>
   <si>
@@ -83,31 +74,13 @@
     <t>Pruebas realizadas</t>
   </si>
   <si>
-    <t xml:space="preserve">Descripción de las pruebas funcionales realizadas. </t>
-  </si>
-  <si>
     <t>Resultados</t>
   </si>
   <si>
-    <t xml:space="preserve">Resultados de las pruebas funcionales. </t>
-  </si>
-  <si>
     <t>Pruebas de Rendimiento</t>
   </si>
   <si>
-    <t xml:space="preserve">Descripción de las pruebas de rendimiento realizadas. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resultados de las pruebas de rendimiento. </t>
-  </si>
-  <si>
     <t>Pruebas seguridad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción de las pruebas de seguridad realizadas. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resultados de las pruebas de seguridad. </t>
   </si>
   <si>
     <r>
@@ -134,32 +107,59 @@
     <t>Problemas</t>
   </si>
   <si>
-    <t xml:space="preserve"> [Descripción del problema identificado] </t>
-  </si>
-  <si>
     <t>Estado</t>
   </si>
   <si>
-    <t xml:space="preserve"> [Abierto/Cerrado]</t>
-  </si>
-  <si>
     <t>Acciones Correctivas</t>
   </si>
   <si>
-    <t>[Acciones tomadas para corregir el problema]</t>
-  </si>
-  <si>
     <t>PRUEBAS</t>
   </si>
   <si>
     <t>1/1</t>
+  </si>
+  <si>
+    <t>Nicolás Barcia Quintela</t>
+  </si>
+  <si>
+    <t>nicolas.barcia@rai.usc.es</t>
+  </si>
+  <si>
+    <t>NBQ_050100</t>
+  </si>
+  <si>
+    <t>Se realizaron pruebas unitarias y de integración para verificar la correcta generación del PDF, incluyendo la precisión del contenido exportado, el formato y la accesibilidad.</t>
+  </si>
+  <si>
+    <t>Todas las pruebas funcionales pasaron exitosamente. Se validó la precisión del contenido y la accesibilidad según estándares.</t>
+  </si>
+  <si>
+    <t>Se llevaron a cabo pruebas de carga para evaluar la funcionalidad con grandes volúmenes de datos, abarcando distintos tamaños de grupos de gasto.</t>
+  </si>
+  <si>
+    <t>Las pruebas indicaron un rendimiento adecuado para grupos de tamaño de todo tipo. Con grandes volúmenes de datos se observan mayores tiempos de carga, pero dentro de cantidades asumibles.</t>
+  </si>
+  <si>
+    <t>Se realizaron análisis de vulnerabilidades, pruebas de penetración y revisión de la privacidad de datos.</t>
+  </si>
+  <si>
+    <t>No se encontraron vulnerabilidades críticas. Demuestra una buena resistencia contra ataques simulados gracias a medidas de validación de entrada y encriptación de datos. Se confirma la adecuación de las prácticas de manejo y protección de datos.</t>
+  </si>
+  <si>
+    <t>No se han identificado problemas.</t>
+  </si>
+  <si>
+    <t>Cerrado</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -283,6 +283,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -671,10 +679,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -688,18 +697,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -713,12 +710,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -729,12 +720,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -742,168 +727,54 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -916,8 +787,165 @@
     <xf numFmtId="16" fontId="17" fillId="2" borderId="34" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -934,9 +962,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -974,7 +1002,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1080,7 +1108,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1222,7 +1250,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1232,16 +1260,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1B85DD8-8EC6-4385-8068-0606E84EE1C9}">
   <dimension ref="D3:K50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:11" ht="15.75" thickBot="1"/>
+    <row r="3" spans="4:11" ht="15" thickBot="1"/>
     <row r="4" spans="4:11">
       <c r="D4" s="1" t="s">
         <v>0</v>
@@ -1256,530 +1284,556 @@
         <v>2</v>
       </c>
       <c r="J4" s="5">
-        <v>45323</v>
+        <v>45349</v>
       </c>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" spans="4:11" ht="15.75" thickBot="1">
-      <c r="D5" s="7" t="s">
+    <row r="5" spans="4:11" ht="15" thickBot="1">
+      <c r="D5" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="9" t="s">
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="10"/>
-    </row>
-    <row r="6" spans="4:11" ht="15.75" hidden="1" thickBot="1">
-      <c r="D6" s="11"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="15"/>
+      <c r="I5" s="69"/>
+      <c r="J5" s="69"/>
+      <c r="K5" s="70"/>
+    </row>
+    <row r="6" spans="4:11" ht="15" hidden="1" thickBot="1">
+      <c r="D6" s="7"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="11"/>
     </row>
     <row r="7" spans="4:11">
-      <c r="D7" s="16"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="21"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="72"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="15"/>
     </row>
     <row r="8" spans="4:11">
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="25"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="60"/>
+      <c r="G8" s="66"/>
+      <c r="H8" s="66"/>
+      <c r="I8" s="66"/>
+      <c r="J8" s="66"/>
+      <c r="K8" s="17"/>
     </row>
     <row r="9" spans="4:11">
-      <c r="D9" s="26"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="25"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="17"/>
     </row>
     <row r="10" spans="4:11">
-      <c r="D10" s="27" t="s">
+      <c r="D10" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="29" t="s">
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="73" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="74"/>
+      <c r="I10" s="74"/>
+      <c r="J10" s="75"/>
+      <c r="K10" s="19"/>
+    </row>
+    <row r="11" spans="4:11">
+      <c r="D11" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="32"/>
-    </row>
-    <row r="11" spans="4:11">
-      <c r="D11" s="33" t="s">
+      <c r="E11" s="55"/>
+      <c r="F11" s="55"/>
+      <c r="G11" s="76" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="58"/>
+      <c r="I11" s="58"/>
+      <c r="J11" s="59"/>
+      <c r="K11" s="20"/>
+    </row>
+    <row r="12" spans="4:11">
+      <c r="D12" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="35" t="s">
+      <c r="E12" s="60"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="61" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="62"/>
+      <c r="I12" s="62"/>
+      <c r="J12" s="63"/>
+      <c r="K12" s="20"/>
+    </row>
+    <row r="13" spans="4:11">
+      <c r="D13" s="21"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="24"/>
+    </row>
+    <row r="14" spans="4:11">
+      <c r="D14" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="H11" s="36"/>
-      <c r="I11" s="36"/>
-      <c r="J11" s="37"/>
-      <c r="K11" s="38"/>
-    </row>
-    <row r="12" spans="4:11">
-      <c r="D12" s="27" t="s">
+      <c r="E14" s="65"/>
+      <c r="F14" s="65"/>
+      <c r="G14" s="66"/>
+      <c r="H14" s="66"/>
+      <c r="I14" s="66"/>
+      <c r="J14" s="66"/>
+      <c r="K14" s="17"/>
+    </row>
+    <row r="15" spans="4:11">
+      <c r="D15" s="25"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="17"/>
+    </row>
+    <row r="16" spans="4:11">
+      <c r="D16" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="39" t="s">
-        <v>11</v>
-      </c>
-      <c r="H12" s="40"/>
-      <c r="I12" s="40"/>
-      <c r="J12" s="41"/>
-      <c r="K12" s="38"/>
-    </row>
-    <row r="13" spans="4:11">
-      <c r="D13" s="42"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="44"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="44"/>
-      <c r="K13" s="45"/>
-    </row>
-    <row r="14" spans="4:11">
-      <c r="D14" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="46"/>
-      <c r="F14" s="46"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="24"/>
-      <c r="J14" s="24"/>
-      <c r="K14" s="25"/>
-    </row>
-    <row r="15" spans="4:11">
-      <c r="D15" s="47"/>
-      <c r="G15" s="48"/>
-      <c r="H15" s="48"/>
-      <c r="I15" s="48"/>
-      <c r="J15" s="48"/>
-      <c r="K15" s="25"/>
-    </row>
-    <row r="16" spans="4:11">
-      <c r="D16" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="48"/>
-      <c r="H16" s="48"/>
-      <c r="I16" s="48"/>
-      <c r="J16" s="48"/>
-      <c r="K16" s="25"/>
+      <c r="E16" s="55"/>
+      <c r="F16" s="55"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="17"/>
     </row>
     <row r="17" spans="4:11">
-      <c r="D17" s="26"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="48"/>
-      <c r="J17" s="48"/>
-      <c r="K17" s="25"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="17"/>
     </row>
     <row r="18" spans="4:11" ht="15" customHeight="1">
       <c r="D18" s="49" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E18" s="50"/>
       <c r="F18" s="51"/>
-      <c r="G18" s="52" t="s">
-        <v>15</v>
-      </c>
-      <c r="H18" s="53"/>
-      <c r="I18" s="53"/>
-      <c r="J18" s="54"/>
-      <c r="K18" s="25"/>
+      <c r="G18" s="77" t="s">
+        <v>24</v>
+      </c>
+      <c r="H18" s="78"/>
+      <c r="I18" s="78"/>
+      <c r="J18" s="79"/>
+      <c r="K18" s="17"/>
     </row>
     <row r="19" spans="4:11">
-      <c r="D19" s="55"/>
-      <c r="E19" s="56"/>
-      <c r="F19" s="56"/>
-      <c r="G19" s="57"/>
-      <c r="H19" s="58"/>
-      <c r="I19" s="58"/>
-      <c r="J19" s="59"/>
-      <c r="K19" s="25"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="80"/>
+      <c r="H19" s="81"/>
+      <c r="I19" s="81"/>
+      <c r="J19" s="82"/>
+      <c r="K19" s="17"/>
     </row>
     <row r="20" spans="4:11">
-      <c r="D20" s="55"/>
-      <c r="E20" s="56"/>
-      <c r="F20" s="56"/>
-      <c r="G20" s="60"/>
-      <c r="H20" s="60"/>
-      <c r="I20" s="60"/>
-      <c r="J20" s="60"/>
-      <c r="K20" s="25"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="17"/>
     </row>
     <row r="21" spans="4:11" ht="15" customHeight="1">
       <c r="D21" s="49" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E21" s="50"/>
       <c r="F21" s="51"/>
-      <c r="G21" s="61" t="s">
-        <v>17</v>
-      </c>
-      <c r="H21" s="62"/>
-      <c r="I21" s="62"/>
-      <c r="J21" s="63"/>
-      <c r="K21" s="25"/>
-    </row>
-    <row r="22" spans="4:11">
-      <c r="D22" s="55"/>
-      <c r="E22" s="56"/>
-      <c r="F22" s="56"/>
-      <c r="G22" s="64"/>
-      <c r="H22" s="65"/>
-      <c r="I22" s="65"/>
-      <c r="J22" s="66"/>
-      <c r="K22" s="25"/>
+      <c r="G21" s="83" t="s">
+        <v>25</v>
+      </c>
+      <c r="H21" s="84"/>
+      <c r="I21" s="84"/>
+      <c r="J21" s="85"/>
+      <c r="K21" s="17"/>
+    </row>
+    <row r="22" spans="4:11" ht="18.600000000000001" customHeight="1">
+      <c r="D22" s="27"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="86"/>
+      <c r="H22" s="87"/>
+      <c r="I22" s="87"/>
+      <c r="J22" s="88"/>
+      <c r="K22" s="17"/>
     </row>
     <row r="23" spans="4:11">
-      <c r="D23" s="55"/>
-      <c r="E23" s="56"/>
-      <c r="F23" s="56"/>
-      <c r="G23" s="60"/>
-      <c r="H23" s="60"/>
-      <c r="I23" s="60"/>
-      <c r="J23" s="60"/>
-      <c r="K23" s="25"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="17"/>
     </row>
     <row r="24" spans="4:11">
-      <c r="D24" s="67" t="s">
-        <v>18</v>
-      </c>
-      <c r="E24" s="68"/>
-      <c r="F24" s="68"/>
-      <c r="G24" s="69"/>
-      <c r="H24" s="69"/>
-      <c r="I24" s="69"/>
-      <c r="J24" s="69"/>
-      <c r="K24" s="70"/>
+      <c r="D24" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="57"/>
+      <c r="F24" s="57"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="29"/>
+      <c r="K24" s="30"/>
     </row>
     <row r="25" spans="4:11">
-      <c r="D25" s="55"/>
-      <c r="E25" s="56"/>
-      <c r="F25" s="56"/>
-      <c r="G25" s="60"/>
-      <c r="H25" s="60"/>
-      <c r="I25" s="60"/>
-      <c r="J25" s="60"/>
-      <c r="K25" s="25"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="17"/>
     </row>
     <row r="26" spans="4:11" ht="15" customHeight="1">
       <c r="D26" s="49" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E26" s="50"/>
       <c r="F26" s="51"/>
-      <c r="G26" s="71" t="s">
-        <v>19</v>
-      </c>
-      <c r="H26" s="72"/>
-      <c r="I26" s="72"/>
-      <c r="J26" s="73"/>
-      <c r="K26" s="25"/>
+      <c r="G26" s="89" t="s">
+        <v>26</v>
+      </c>
+      <c r="H26" s="90"/>
+      <c r="I26" s="90"/>
+      <c r="J26" s="91"/>
+      <c r="K26" s="17"/>
     </row>
     <row r="27" spans="4:11">
-      <c r="D27" s="55"/>
-      <c r="E27" s="56"/>
-      <c r="F27" s="56"/>
-      <c r="G27" s="74"/>
-      <c r="H27" s="75"/>
-      <c r="I27" s="75"/>
-      <c r="J27" s="76"/>
-      <c r="K27" s="25"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="92"/>
+      <c r="H27" s="93"/>
+      <c r="I27" s="93"/>
+      <c r="J27" s="94"/>
+      <c r="K27" s="17"/>
     </row>
     <row r="28" spans="4:11">
-      <c r="D28" s="55"/>
-      <c r="E28" s="56"/>
-      <c r="F28" s="56"/>
-      <c r="G28" s="77"/>
-      <c r="H28" s="77"/>
-      <c r="I28" s="77"/>
-      <c r="J28" s="77"/>
-      <c r="K28" s="25"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="31"/>
+      <c r="H28" s="31"/>
+      <c r="I28" s="31"/>
+      <c r="J28" s="31"/>
+      <c r="K28" s="17"/>
     </row>
     <row r="29" spans="4:11">
-      <c r="D29" s="55"/>
+      <c r="D29" s="27"/>
       <c r="E29" s="50" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F29" s="50"/>
-      <c r="G29" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="H29" s="62"/>
-      <c r="I29" s="62"/>
-      <c r="J29" s="63"/>
-      <c r="K29" s="25"/>
-    </row>
-    <row r="30" spans="4:11">
-      <c r="D30" s="55"/>
-      <c r="E30" s="78"/>
-      <c r="F30" s="78"/>
-      <c r="G30" s="64"/>
-      <c r="H30" s="65"/>
-      <c r="I30" s="65"/>
-      <c r="J30" s="66"/>
-      <c r="K30" s="25"/>
+      <c r="G29" s="83" t="s">
+        <v>27</v>
+      </c>
+      <c r="H29" s="84"/>
+      <c r="I29" s="84"/>
+      <c r="J29" s="85"/>
+      <c r="K29" s="17"/>
+    </row>
+    <row r="30" spans="4:11" ht="36.6" customHeight="1">
+      <c r="D30" s="27"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="86"/>
+      <c r="H30" s="87"/>
+      <c r="I30" s="87"/>
+      <c r="J30" s="88"/>
+      <c r="K30" s="17"/>
     </row>
     <row r="31" spans="4:11">
-      <c r="D31" s="55"/>
-      <c r="E31" s="56"/>
-      <c r="F31" s="56"/>
-      <c r="G31" s="60"/>
-      <c r="H31" s="60"/>
-      <c r="I31" s="60"/>
-      <c r="J31" s="60"/>
-      <c r="K31" s="25"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="16"/>
+      <c r="K31" s="17"/>
     </row>
     <row r="32" spans="4:11">
-      <c r="D32" s="79" t="s">
-        <v>21</v>
-      </c>
-      <c r="E32" s="80"/>
-      <c r="F32" s="80"/>
-      <c r="G32" s="69"/>
-      <c r="H32" s="69"/>
-      <c r="I32" s="69"/>
-      <c r="J32" s="69"/>
-      <c r="K32" s="70"/>
+      <c r="D32" s="52" t="s">
+        <v>14</v>
+      </c>
+      <c r="E32" s="53"/>
+      <c r="F32" s="53"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="29"/>
+      <c r="I32" s="29"/>
+      <c r="J32" s="29"/>
+      <c r="K32" s="30"/>
     </row>
     <row r="33" spans="4:11">
-      <c r="D33" s="55"/>
-      <c r="E33" s="56"/>
-      <c r="F33" s="56"/>
-      <c r="G33" s="60"/>
-      <c r="H33" s="60"/>
-      <c r="I33" s="60"/>
-      <c r="J33" s="60"/>
-      <c r="K33" s="25"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="16"/>
+      <c r="K33" s="17"/>
     </row>
     <row r="34" spans="4:11" ht="15" customHeight="1">
       <c r="D34" s="49" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E34" s="50"/>
       <c r="F34" s="51"/>
-      <c r="G34" s="71" t="s">
-        <v>22</v>
-      </c>
-      <c r="H34" s="72"/>
-      <c r="I34" s="72"/>
-      <c r="J34" s="73"/>
-      <c r="K34" s="25"/>
+      <c r="G34" s="89" t="s">
+        <v>28</v>
+      </c>
+      <c r="H34" s="90"/>
+      <c r="I34" s="90"/>
+      <c r="J34" s="91"/>
+      <c r="K34" s="17"/>
     </row>
     <row r="35" spans="4:11">
-      <c r="D35" s="55"/>
-      <c r="E35" s="78"/>
-      <c r="F35" s="78"/>
-      <c r="G35" s="74"/>
-      <c r="H35" s="75"/>
-      <c r="I35" s="75"/>
-      <c r="J35" s="76"/>
-      <c r="K35" s="25"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="32"/>
+      <c r="G35" s="92"/>
+      <c r="H35" s="93"/>
+      <c r="I35" s="93"/>
+      <c r="J35" s="94"/>
+      <c r="K35" s="17"/>
     </row>
     <row r="36" spans="4:11">
-      <c r="D36" s="55"/>
-      <c r="E36" s="56"/>
-      <c r="F36" s="56"/>
-      <c r="G36" s="77"/>
-      <c r="H36" s="77"/>
-      <c r="I36" s="77"/>
-      <c r="J36" s="77"/>
-      <c r="K36" s="25"/>
+      <c r="D36" s="27"/>
+      <c r="E36" s="28"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="31"/>
+      <c r="H36" s="31"/>
+      <c r="I36" s="31"/>
+      <c r="J36" s="31"/>
+      <c r="K36" s="17"/>
     </row>
     <row r="37" spans="4:11" ht="15" customHeight="1">
       <c r="D37" s="49" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E37" s="50"/>
       <c r="F37" s="51"/>
-      <c r="G37" s="61" t="s">
-        <v>23</v>
-      </c>
-      <c r="H37" s="62"/>
-      <c r="I37" s="62"/>
-      <c r="J37" s="63"/>
-      <c r="K37" s="25"/>
-    </row>
-    <row r="38" spans="4:11">
-      <c r="D38" s="55"/>
-      <c r="E38" s="78"/>
-      <c r="F38" s="78"/>
-      <c r="G38" s="64"/>
-      <c r="H38" s="65"/>
-      <c r="I38" s="65"/>
-      <c r="J38" s="66"/>
-      <c r="K38" s="25"/>
+      <c r="G37" s="95" t="s">
+        <v>29</v>
+      </c>
+      <c r="H37" s="96"/>
+      <c r="I37" s="96"/>
+      <c r="J37" s="97"/>
+      <c r="K37" s="17"/>
+    </row>
+    <row r="38" spans="4:11" ht="37.200000000000003" customHeight="1">
+      <c r="D38" s="27"/>
+      <c r="E38" s="32"/>
+      <c r="F38" s="32"/>
+      <c r="G38" s="98"/>
+      <c r="H38" s="99"/>
+      <c r="I38" s="99"/>
+      <c r="J38" s="100"/>
+      <c r="K38" s="17"/>
     </row>
     <row r="39" spans="4:11">
-      <c r="D39" s="55"/>
-      <c r="E39" s="56"/>
-      <c r="F39" s="56"/>
-      <c r="G39" s="60"/>
-      <c r="H39" s="60"/>
-      <c r="I39" s="60"/>
-      <c r="J39" s="60"/>
-      <c r="K39" s="25"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="28"/>
+      <c r="F39" s="28"/>
+      <c r="G39" s="16"/>
+      <c r="H39" s="16"/>
+      <c r="I39" s="16"/>
+      <c r="J39" s="16"/>
+      <c r="K39" s="17"/>
     </row>
     <row r="40" spans="4:11">
-      <c r="D40" s="47"/>
-      <c r="G40" s="48"/>
-      <c r="H40" s="48"/>
-      <c r="I40" s="48"/>
-      <c r="J40" s="48"/>
-      <c r="K40" s="25"/>
+      <c r="D40" s="25"/>
+      <c r="G40" s="26"/>
+      <c r="H40" s="26"/>
+      <c r="I40" s="26"/>
+      <c r="J40" s="26"/>
+      <c r="K40" s="17"/>
     </row>
     <row r="41" spans="4:11">
-      <c r="D41" s="81" t="s">
-        <v>24</v>
-      </c>
-      <c r="E41" s="82"/>
-      <c r="F41" s="83"/>
-      <c r="G41" s="69"/>
-      <c r="H41" s="69"/>
-      <c r="I41" s="69"/>
-      <c r="J41" s="69"/>
-      <c r="K41" s="70"/>
+      <c r="D41" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="E41" s="34"/>
+      <c r="F41" s="35"/>
+      <c r="G41" s="29"/>
+      <c r="H41" s="29"/>
+      <c r="I41" s="29"/>
+      <c r="J41" s="29"/>
+      <c r="K41" s="30"/>
     </row>
     <row r="42" spans="4:11">
-      <c r="D42" s="47"/>
-      <c r="G42" s="48"/>
-      <c r="H42" s="48"/>
-      <c r="I42" s="48"/>
-      <c r="J42" s="48"/>
-      <c r="K42" s="25"/>
+      <c r="D42" s="25"/>
+      <c r="G42" s="26"/>
+      <c r="H42" s="26"/>
+      <c r="I42" s="26"/>
+      <c r="J42" s="26"/>
+      <c r="K42" s="17"/>
     </row>
     <row r="43" spans="4:11">
-      <c r="D43" s="47"/>
-      <c r="E43" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="F43" s="28"/>
-      <c r="G43" s="84" t="s">
-        <v>26</v>
-      </c>
-      <c r="H43" s="85"/>
-      <c r="I43" s="85"/>
-      <c r="J43" s="86"/>
-      <c r="K43" s="25"/>
+      <c r="D43" s="25"/>
+      <c r="E43" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="F43" s="41"/>
+      <c r="G43" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="H43" s="43"/>
+      <c r="I43" s="43"/>
+      <c r="J43" s="44"/>
+      <c r="K43" s="17"/>
     </row>
     <row r="44" spans="4:11">
-      <c r="D44" s="47"/>
-      <c r="G44" s="48"/>
-      <c r="H44" s="48"/>
-      <c r="I44" s="48"/>
-      <c r="J44" s="48"/>
-      <c r="K44" s="25"/>
+      <c r="D44" s="25"/>
+      <c r="G44" s="26"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="26"/>
+      <c r="J44" s="26"/>
+      <c r="K44" s="17"/>
     </row>
     <row r="45" spans="4:11">
-      <c r="D45" s="47"/>
-      <c r="E45" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="F45" s="28"/>
-      <c r="G45" s="84" t="s">
-        <v>28</v>
-      </c>
-      <c r="H45" s="85"/>
-      <c r="I45" s="85"/>
-      <c r="J45" s="86"/>
-      <c r="K45" s="25"/>
+      <c r="D45" s="25"/>
+      <c r="E45" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="F45" s="41"/>
+      <c r="G45" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="H45" s="43"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="44"/>
+      <c r="K45" s="17"/>
     </row>
     <row r="46" spans="4:11">
-      <c r="D46" s="47"/>
-      <c r="F46" s="87"/>
-      <c r="G46" s="48"/>
-      <c r="H46" s="48"/>
-      <c r="I46" s="48"/>
-      <c r="J46" s="48"/>
-      <c r="K46" s="25"/>
+      <c r="D46" s="25"/>
+      <c r="F46" s="36"/>
+      <c r="G46" s="26"/>
+      <c r="H46" s="26"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
+      <c r="K46" s="17"/>
     </row>
     <row r="47" spans="4:11">
-      <c r="D47" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="E47" s="28"/>
-      <c r="F47" s="28"/>
-      <c r="G47" s="84" t="s">
-        <v>30</v>
-      </c>
-      <c r="H47" s="85"/>
-      <c r="I47" s="85"/>
-      <c r="J47" s="86"/>
-      <c r="K47" s="25"/>
+      <c r="D47" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="E47" s="41"/>
+      <c r="F47" s="41"/>
+      <c r="G47" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="H47" s="43"/>
+      <c r="I47" s="43"/>
+      <c r="J47" s="44"/>
+      <c r="K47" s="17"/>
     </row>
     <row r="48" spans="4:11">
-      <c r="D48" s="47"/>
-      <c r="F48" s="87"/>
-      <c r="G48" s="48"/>
-      <c r="H48" s="48"/>
-      <c r="I48" s="48"/>
-      <c r="J48" s="48"/>
-      <c r="K48" s="25"/>
-    </row>
-    <row r="49" spans="4:11" ht="15.75" thickBot="1">
-      <c r="D49" s="88"/>
-      <c r="E49" s="89"/>
-      <c r="F49" s="89"/>
-      <c r="G49" s="89"/>
-      <c r="H49" s="89"/>
-      <c r="I49" s="89"/>
-      <c r="J49" s="89"/>
-      <c r="K49" s="90"/>
-    </row>
-    <row r="50" spans="4:11" ht="15.75" thickBot="1">
-      <c r="D50" s="91" t="s">
-        <v>31</v>
-      </c>
-      <c r="E50" s="92"/>
-      <c r="F50" s="92"/>
-      <c r="G50" s="92"/>
-      <c r="H50" s="92"/>
-      <c r="I50" s="92"/>
-      <c r="J50" s="93" t="s">
-        <v>32</v>
-      </c>
-      <c r="K50" s="94"/>
+      <c r="D48" s="25"/>
+      <c r="F48" s="36"/>
+      <c r="G48" s="26"/>
+      <c r="H48" s="26"/>
+      <c r="I48" s="26"/>
+      <c r="J48" s="26"/>
+      <c r="K48" s="17"/>
+    </row>
+    <row r="49" spans="4:11" ht="15" thickBot="1">
+      <c r="D49" s="37"/>
+      <c r="E49" s="38"/>
+      <c r="F49" s="38"/>
+      <c r="G49" s="38"/>
+      <c r="H49" s="38"/>
+      <c r="I49" s="38"/>
+      <c r="J49" s="38"/>
+      <c r="K49" s="39"/>
+    </row>
+    <row r="50" spans="4:11" ht="15" thickBot="1">
+      <c r="D50" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="E50" s="46"/>
+      <c r="F50" s="46"/>
+      <c r="G50" s="46"/>
+      <c r="H50" s="46"/>
+      <c r="I50" s="46"/>
+      <c r="J50" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="K50" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="G8:J8"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="G11:J11"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="G12:J12"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="G34:J35"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="G18:J19"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="G21:J22"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="G26:J27"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="G29:J30"/>
+    <mergeCell ref="D32:F32"/>
     <mergeCell ref="D47:F47"/>
     <mergeCell ref="G47:J47"/>
     <mergeCell ref="D50:I50"/>
@@ -1790,33 +1844,10 @@
     <mergeCell ref="G43:J43"/>
     <mergeCell ref="E45:F45"/>
     <mergeCell ref="G45:J45"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="G26:J27"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="G29:J30"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="G34:J35"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="G18:J19"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="G21:J22"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="G11:J11"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="G12:J12"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="G8:J8"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="G10:J10"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="G11" r:id="rId1" xr:uid="{6CE98F42-4380-46B6-B13F-3395F2D79559}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>